<commit_message>
updating score board format and placing sample data
</commit_message>
<xml_diff>
--- a/Local_Files/Score_Boards.xlsx
+++ b/Local_Files/Score_Boards.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytnstate-my.sharepoint.com/personal/afolorun_my_tnstate_edu/Documents/Technical/Personal Projects/WordGame/Local_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{17B2720E-1FA2-4E1E-85DF-0F9BB15B4DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A80CB74-EDA1-40C0-93EF-5E9B498AD3C4}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{17B2720E-1FA2-4E1E-85DF-0F9BB15B4DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA01A4B9-F758-45E0-80B3-92BCC9E7091F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA590432-5F41-4DA7-8836-A3E94E47CCF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EA590432-5F41-4DA7-8836-A3E94E47CCF4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Classic Scores" sheetId="1" r:id="rId1"/>
-    <sheet name="Hangman Scores" sheetId="2" r:id="rId2"/>
+    <sheet name="Top Scores" sheetId="3" r:id="rId1"/>
+    <sheet name="Classic Scores" sheetId="1" r:id="rId2"/>
+    <sheet name="Hangman Scores" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,9 +38,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>H</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Game mode</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>Hangman</t>
+  </si>
+  <si>
+    <t>"Normal"</t>
+  </si>
+  <si>
+    <t>"Easy"</t>
+  </si>
+  <si>
+    <t>"Hard"</t>
+  </si>
+  <si>
+    <t>"Ultra_Hard"</t>
   </si>
 </sst>
 </file>
@@ -92,6 +120,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,28 +442,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF8801E-77C2-423F-9B9E-D218300B70E8}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EAAA7F-4DA9-4A3D-9653-E3C06645F9E9}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA90C9B-E1FE-4F36-A7D4-AB5FC9CCC2AF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF8801E-77C2-423F-9B9E-D218300B70E8}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA90C9B-E1FE-4F36-A7D4-AB5FC9CCC2AF}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>